<commit_message>
TestReport after login Restructure
Test report Ok
</commit_message>
<xml_diff>
--- a/TestingAndCalibrationLabs/TestingAndCalibrationLabs/TestCases (1).xlsx
+++ b/TestingAndCalibrationLabs/TestingAndCalibrationLabs/TestCases (1).xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa2e4abb4efb2a86/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SumanthCSSRestructuringLogin\TestingAndCalibrationLabs\TestingAndCalibrationLabs\TestingAndCalibrationLabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{E36EFD56-2832-4012-A19E-7DD5EDE8BE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FE1468-17F2-4436-A766-685F1E1D701B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5740616-BAD6-46C7-B24B-C4CDD780B2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="0" windowWidth="11904" windowHeight="11376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Restructure" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="128">
   <si>
     <t>Test Cases</t>
   </si>
@@ -192,17 +193,242 @@
   </si>
   <si>
     <t>It does not redirect to view list on click</t>
+  </si>
+  <si>
+    <t>Normal Load In Pc View</t>
+  </si>
+  <si>
+    <t>Noramlly as expected</t>
+  </si>
+  <si>
+    <t>In Mid Screen</t>
+  </si>
+  <si>
+    <t>In Mobile Screen</t>
+  </si>
+  <si>
+    <t>Submit Button</t>
+  </si>
+  <si>
+    <t>Same As everywhere in the project</t>
+  </si>
+  <si>
+    <t>FOOTER</t>
+  </si>
+  <si>
+    <t>at the bottom of screen</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other character visible </t>
+  </si>
+  <si>
+    <t>Not expected</t>
+  </si>
+  <si>
+    <t>Menu in PC view</t>
+  </si>
+  <si>
+    <t>visible and fine</t>
+  </si>
+  <si>
+    <t>Menu in Mid, Small Screen</t>
+  </si>
+  <si>
+    <t>three bars visible and collapasable</t>
+  </si>
+  <si>
+    <t>Progress screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visisbile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snack Bar message </t>
+  </si>
+  <si>
+    <t>Filelds Inputs</t>
+  </si>
+  <si>
+    <t>Name (Alphanumeric)</t>
+  </si>
+  <si>
+    <t>Accepting AlphaNumeric Only</t>
+  </si>
+  <si>
+    <t>EmailId(Alphanumeric)</t>
+  </si>
+  <si>
+    <t>Mobile Number (Numeric)</t>
+  </si>
+  <si>
+    <t>Accepting Numeric Only</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Pin Code</t>
+  </si>
+  <si>
+    <t>Testing Type</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>SURVEY</t>
+  </si>
+  <si>
+    <t>TestDetailsGrid</t>
+  </si>
+  <si>
+    <t>Input Fields of TestGrid</t>
+  </si>
+  <si>
+    <t>Job Serial no (Numeric)</t>
+  </si>
+  <si>
+    <t>Departmet Name (Alphanumeric)</t>
+  </si>
+  <si>
+    <t>Customer Name (Alphanumeric)</t>
+  </si>
+  <si>
+    <t>Issue To</t>
+  </si>
+  <si>
+    <t>Received On</t>
+  </si>
+  <si>
+    <t>Job Order</t>
+  </si>
+  <si>
+    <t>Contact Person</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Test Report Release date</t>
+  </si>
+  <si>
+    <t>Any Other</t>
+  </si>
+  <si>
+    <t>File Attach</t>
+  </si>
+  <si>
+    <t>Data Grid</t>
+  </si>
+  <si>
+    <t>Tree Select</t>
+  </si>
+  <si>
+    <t>Date dd-mm-yyy</t>
+  </si>
+  <si>
+    <t>Shows Data</t>
+  </si>
+  <si>
+    <t>Hard Coated</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No field validation </t>
+  </si>
+  <si>
+    <t>It is absent</t>
+  </si>
+  <si>
+    <t>Showing the number of file attached</t>
+  </si>
+  <si>
+    <t>Shows number of Files</t>
+  </si>
+  <si>
+    <t>TestGrid in Pc View</t>
+  </si>
+  <si>
+    <t>should show data properly</t>
+  </si>
+  <si>
+    <t>TestGrid In Mobile View</t>
+  </si>
+  <si>
+    <t>should show data properly in the screen</t>
+  </si>
+  <si>
+    <t>Grid is scrollable in Mobile view</t>
+  </si>
+  <si>
+    <t>to view all data it should be scrollable</t>
+  </si>
+  <si>
+    <t>Login "SignIn"</t>
+  </si>
+  <si>
+    <t>Ui appearance in Pc view</t>
+  </si>
+  <si>
+    <t>Ui appearance in Mid Screen view</t>
+  </si>
+  <si>
+    <t>Ui appearance in Mobile Screen view</t>
+  </si>
+  <si>
+    <t>It should appear properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position of Buttons </t>
+  </si>
+  <si>
+    <t>It shold be at appropriate place</t>
+  </si>
+  <si>
+    <t>Position of socail buttons</t>
+  </si>
+  <si>
+    <t>Remember me checkbox</t>
+  </si>
+  <si>
+    <t>It should put a tick on click and disappear on next click</t>
+  </si>
+  <si>
+    <t>Login "SignUP"</t>
+  </si>
+  <si>
+    <t>Social buttons Icon looks ok</t>
+  </si>
+  <si>
+    <t>Login SingIn SignUP</t>
+  </si>
+  <si>
+    <t>visisble after submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Icon is misplaced </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -210,24 +436,69 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -242,13 +513,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="52"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,22 +832,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="63.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.796875" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="5" max="5" width="63.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -563,7 +864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -574,7 +875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -582,7 +883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -596,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -610,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="A6">
         <v>2.2999999999999998</v>
       </c>
@@ -618,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7">
         <v>2.4</v>
       </c>
@@ -635,7 +936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8">
         <v>2.5</v>
       </c>
@@ -649,7 +950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9">
         <v>2.6</v>
       </c>
@@ -666,7 +967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10">
         <v>2.7</v>
       </c>
@@ -683,7 +984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="A11">
         <v>2.8</v>
       </c>
@@ -697,7 +998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12">
         <v>2.9</v>
       </c>
@@ -711,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -725,7 +1026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
@@ -734,11 +1035,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -752,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2.8</v>
       </c>
@@ -766,7 +1067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2.9</v>
       </c>
@@ -783,12 +1084,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="D19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>3</v>
       </c>
@@ -802,7 +1103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>3.1</v>
       </c>
@@ -816,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>3.2</v>
       </c>
@@ -830,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>4</v>
       </c>
@@ -844,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>5</v>
       </c>
@@ -861,7 +1162,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>6</v>
       </c>
@@ -882,4 +1183,714 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC131F17-3B20-43CB-B84C-7F0FAFA4604A}">
+  <dimension ref="A1:E80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="28.19921875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.19921875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="29.09765625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="47.3984375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" ht="19.95" customHeight="1">
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="E62" s="13"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="13"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="13"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="13"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="13"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="13"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="E70" s="13"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="E71" s="13"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="E72" s="13"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E73" s="13"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="13"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="13"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="13"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="13"/>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="13"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="E79" s="13"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E2:E29"/>
+    <mergeCell ref="E31:E46"/>
+    <mergeCell ref="E61:E80"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>